<commit_message>
Prioritization based on task number working correctly
</commit_message>
<xml_diff>
--- a/J301_1_Manual_Calcs.xlsx
+++ b/J301_1_Manual_Calcs.xlsx
@@ -18,6 +18,8 @@
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -182,11 +184,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -208,25 +209,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -253,7 +235,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,29 +259,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -308,17 +274,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading 1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result 3" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2 4" xfId="23" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -446,16 +408,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.62790697674419"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.75348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.01395348837209"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.73953488372093"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="2.58604651162791"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.84651162790698"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.58604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,8 +1337,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,22 +1784,22 @@
   </sheetPr>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.62790697674419"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.75348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.01395348837209"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="2.95348837209302"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.6"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.95348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="3.07441860465116"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="3.07441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2821,17 +2782,15 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topRight" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.62790697674419"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.75348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5245,17 +5204,15 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B34" activeCellId="0" sqref="B34"/>
+      <selection pane="topRight" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.62790697674419"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.75348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5551,7 +5508,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -5573,19 +5530,19 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; I$1,$C$2:$C$33,"&gt;" &amp; I$1)</f>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="J2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; J$1,$C$2:$C$33,"&gt;" &amp; J$1)</f>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="K2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; K$1,$C$2:$C$33,"&gt;" &amp; K$1)</f>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="L2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; L$1,$C$2:$C$33,"&gt;" &amp; L$1)</f>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="M2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; M$1,$C$2:$C$33,"&gt;" &amp; M$1)</f>
@@ -5605,31 +5562,31 @@
       </c>
       <c r="Q2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; Q$1,$C$2:$C$33,"&gt;" &amp; Q$1)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; R$1,$C$2:$C$33,"&gt;" &amp; R$1)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="S2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; S$1,$C$2:$C$33,"&gt;" &amp; S$1)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="T2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; T$1,$C$2:$C$33,"&gt;" &amp; T$1)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="U2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="V2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="W2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; W$1,$C$2:$C$33,"&gt;" &amp; W$1)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; X$1,$C$2:$C$33,"&gt;" &amp; X$1)</f>
@@ -5641,59 +5598,59 @@
       </c>
       <c r="Z2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AA2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AB2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AC2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AD2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AF2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AG2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AH2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AI2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AJ2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
@@ -5729,23 +5686,23 @@
       </c>
       <c r="AV2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AX2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
@@ -5757,35 +5714,35 @@
       </c>
       <c r="BC2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="BD2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="BE2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BF2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BG2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BG$1,$C$2:$C$33,"&gt;" &amp; BG$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BH2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BH$1,$C$2:$C$33,"&gt;" &amp; BH$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BI2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BI$1,$C$2:$C$33,"&gt;" &amp; BI$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BJ2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BJ$1,$C$2:$C$33,"&gt;" &amp; BJ$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BK2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BK$1,$C$2:$C$33,"&gt;" &amp; BK$1)</f>
@@ -5936,7 +5893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -5974,91 +5931,91 @@
       </c>
       <c r="M3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; M$1,$C$2:$C$33,"&gt;" &amp; M$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; N$1,$C$2:$C$33,"&gt;" &amp; N$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; O$1,$C$2:$C$33,"&gt;" &amp; O$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; P$1,$C$2:$C$33,"&gt;" &amp; P$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; Q$1,$C$2:$C$33,"&gt;" &amp; Q$1)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; R$1,$C$2:$C$33,"&gt;" &amp; R$1)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; S$1,$C$2:$C$33,"&gt;" &amp; S$1)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="T3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; T$1,$C$2:$C$33,"&gt;" &amp; T$1)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="V3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; W$1,$C$2:$C$33,"&gt;" &amp; W$1)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="X3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; X$1,$C$2:$C$33,"&gt;" &amp; X$1)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="Y3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; Y$1,$C$2:$C$33,"&gt;" &amp; Y$1)</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="Z3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="AA3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="AB3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AC3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AD3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AF3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AG3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AH3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AI3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
@@ -6086,7 +6043,7 @@
       </c>
       <c r="AO3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AP3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
@@ -6114,23 +6071,23 @@
       </c>
       <c r="AV3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AW3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AX3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AY3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AZ3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BA3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
@@ -6142,23 +6099,23 @@
       </c>
       <c r="BC3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="BD3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="BE3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BF3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BG3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BG$1,$C$2:$C$33,"&gt;" &amp; BG$1)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BH3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BH$1,$C$2:$C$33,"&gt;" &amp; BH$1)</f>
@@ -6170,23 +6127,23 @@
       </c>
       <c r="BJ3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BJ$1,$C$2:$C$33,"&gt;" &amp; BJ$1)</f>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="BK3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BK$1,$C$2:$C$33,"&gt;" &amp; BK$1)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BL3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BL$1,$C$2:$C$33,"&gt;" &amp; BL$1)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BM3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BM$1,$C$2:$C$33,"&gt;" &amp; BM$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BN3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BN$1,$C$2:$C$33,"&gt;" &amp; BN$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BO3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BO$1,$C$2:$C$33,"&gt;" &amp; BO$1)</f>
@@ -6321,16 +6278,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">B4+Constrained_Data!C9</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>1</v>
@@ -6411,23 +6368,23 @@
       </c>
       <c r="Z4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AC4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AE4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
@@ -6439,23 +6396,23 @@
       </c>
       <c r="AG4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AK4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AL4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
@@ -6706,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -6752,31 +6709,31 @@
       </c>
       <c r="O5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; O$1,$C$2:$C$33,"&gt;" &amp; O$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; P$1,$C$2:$C$33,"&gt;" &amp; P$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; Q$1,$C$2:$C$33,"&gt;" &amp; Q$1)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; R$1,$C$2:$C$33,"&gt;" &amp; R$1)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; S$1,$C$2:$C$33,"&gt;" &amp; S$1)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; T$1,$C$2:$C$33,"&gt;" &amp; T$1)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="V5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
@@ -6792,35 +6749,35 @@
       </c>
       <c r="Y5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; Y$1,$C$2:$C$33,"&gt;" &amp; Y$1)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="Z5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AB5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AC5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AD5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AE5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AF5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AG5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
@@ -6832,31 +6789,31 @@
       </c>
       <c r="AI5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AJ5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AK5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AL5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AM5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AN5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AO5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AP5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
@@ -6864,35 +6821,35 @@
       </c>
       <c r="AQ5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AQ$1,$C$2:$C$33,"&gt;" &amp; AQ$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AR5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AR$1,$C$2:$C$33,"&gt;" &amp; AR$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AS5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AS$1,$C$2:$C$33,"&gt;" &amp; AS$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AT5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AT$1,$C$2:$C$33,"&gt;" &amp; AT$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AU5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AU$1,$C$2:$C$33,"&gt;" &amp; AU$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AV5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AW5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="AX5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="AY5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
@@ -6904,23 +6861,23 @@
       </c>
       <c r="BA5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BB5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BC5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BD5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BE5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BF5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
@@ -7096,11 +7053,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">B6+Constrained_Data!C11</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>1</v>
@@ -7132,11 +7089,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">B8+Constrained_Data!C13</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>1</v>
@@ -7150,11 +7107,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">B9+Constrained_Data!C14</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>2</v>
@@ -7168,11 +7125,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">B10+Constrained_Data!C15</f>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>1</v>
@@ -7186,11 +7143,11 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">B11+Constrained_Data!C16</f>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>4</v>
@@ -7204,11 +7161,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">B12+Constrained_Data!C17</f>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>2</v>
@@ -7222,11 +7179,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">B13+Constrained_Data!C18</f>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>2</v>
@@ -7240,11 +7197,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">B14+Constrained_Data!C19</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>1</v>
@@ -7258,11 +7215,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">B15+Constrained_Data!C20</f>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>2</v>
@@ -7276,11 +7233,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">B16+Constrained_Data!C21</f>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>1</v>
@@ -7294,11 +7251,11 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">B17+Constrained_Data!C22</f>
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>4</v>
@@ -7312,11 +7269,11 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">B18+Constrained_Data!C23</f>
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>4</v>
@@ -7330,11 +7287,11 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">B19+Constrained_Data!C24</f>
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>4</v>
@@ -7348,11 +7305,11 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">B20+Constrained_Data!C25</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>2</v>
@@ -7366,11 +7323,11 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">B21+Constrained_Data!C26</f>
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>2</v>
@@ -7384,11 +7341,11 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">B22+Constrained_Data!C27</f>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>4</v>
@@ -7402,11 +7359,11 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">B23+Constrained_Data!C28</f>
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>1</v>
@@ -7420,11 +7377,11 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">B24+Constrained_Data!C29</f>
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>1</v>
@@ -7438,11 +7395,11 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">B25+Constrained_Data!C30</f>
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>2</v>
@@ -7456,11 +7413,11 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">B26+Constrained_Data!C31</f>
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>1</v>
@@ -7474,11 +7431,11 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">B27+Constrained_Data!C32</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>3</v>
@@ -7492,11 +7449,11 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">B28+Constrained_Data!C33</f>
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>4</v>
@@ -7528,11 +7485,11 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">B30+Constrained_Data!C35</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>2</v>
@@ -7546,11 +7503,11 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">B31+Constrained_Data!C36</f>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>2</v>
@@ -7582,11 +7539,11 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">B33+Constrained_Data!C38</f>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Forgot to push yesterday
</commit_message>
<xml_diff>
--- a/J301_1_Manual_Calcs.xlsx
+++ b/J301_1_Manual_Calcs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,9 @@
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -408,16 +410,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.75348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.87441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.13953488372093"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.73953488372093"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="2.58604651162791"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.093023255814"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.58604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1337,7 +1337,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,16 +1791,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.75348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.87441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.13953488372093"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="3.07441860465116"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="3.07441860465116"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="3.2"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="3.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2787,10 +2786,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.75348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.01395348837209"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.87441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.13953488372093"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5202,17 +5202,18 @@
   <dimension ref="A1:CU33"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <pane xSplit="6" ySplit="0" topLeftCell="AG1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topRight" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.75348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.01395348837209"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.87441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.13953488372093"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5578,43 +5579,43 @@
       </c>
       <c r="U2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="V2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="W2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; W$1,$C$2:$C$33,"&gt;" &amp; W$1)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; X$1,$C$2:$C$33,"&gt;" &amp; X$1)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; Y$1,$C$2:$C$33,"&gt;" &amp; Y$1)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Z2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AA2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AB2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AC2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
@@ -5622,35 +5623,35 @@
       </c>
       <c r="AF2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AG2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AH2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AI2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AJ2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AK2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AL2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AM2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AN2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
@@ -5658,71 +5659,71 @@
       </c>
       <c r="AO2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AQ$1,$C$2:$C$33,"&gt;" &amp; AQ$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AR$1,$C$2:$C$33,"&gt;" &amp; AR$1)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AS2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AS$1,$C$2:$C$33,"&gt;" &amp; AS$1)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AT2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AT$1,$C$2:$C$33,"&gt;" &amp; AT$1)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AU2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AU$1,$C$2:$C$33,"&gt;" &amp; AU$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AV2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AW2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AX2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BA2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BB2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BC2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BD2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BE2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BF2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
@@ -5999,11 +6000,11 @@
       </c>
       <c r="AD3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
@@ -6011,47 +6012,47 @@
       </c>
       <c r="AG3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AH3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AI3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AJ3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AK3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AL3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AM3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AN3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AO3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AP3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AQ3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AQ$1,$C$2:$C$33,"&gt;" &amp; AQ$1)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AR3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AR$1,$C$2:$C$33,"&gt;" &amp; AR$1)</f>
@@ -6071,63 +6072,63 @@
       </c>
       <c r="AV3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AW3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AX3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AY3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AZ3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BA3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="BB3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="BC3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BD3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BE3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BF3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BG3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BG$1,$C$2:$C$33,"&gt;" &amp; BG$1)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BH3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BH$1,$C$2:$C$33,"&gt;" &amp; BH$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BI3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BI$1,$C$2:$C$33,"&gt;" &amp; BI$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BJ3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BJ$1,$C$2:$C$33,"&gt;" &amp; BJ$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BK3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BK$1,$C$2:$C$33,"&gt;" &amp; BK$1)</f>
@@ -6488,11 +6489,11 @@
       </c>
       <c r="BD4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BE4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BF4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
@@ -6516,11 +6517,11 @@
       </c>
       <c r="BK4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BK$1,$C$2:$C$33,"&gt;" &amp; BK$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BL4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BL$1,$C$2:$C$33,"&gt;" &amp; BL$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BM4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BM$1,$C$2:$C$33,"&gt;" &amp; BM$1)</f>
@@ -6777,23 +6778,23 @@
       </c>
       <c r="AF5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AG5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AH5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AI5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AJ5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AK5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
@@ -6813,11 +6814,11 @@
       </c>
       <c r="AO5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AP5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AQ5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AQ$1,$C$2:$C$33,"&gt;" &amp; AQ$1)</f>
@@ -6841,11 +6842,11 @@
       </c>
       <c r="AV5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AW5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AX5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
@@ -6853,31 +6854,31 @@
       </c>
       <c r="AY5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AZ5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BA5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BB5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BC5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BD5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BE5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BF5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
@@ -7089,11 +7090,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">B8+Constrained_Data!C13</f>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>1</v>
@@ -7125,11 +7126,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">B10+Constrained_Data!C15</f>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>1</v>
@@ -7197,11 +7198,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">B14+Constrained_Data!C19</f>
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>1</v>
@@ -7233,11 +7234,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">B16+Constrained_Data!C21</f>
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>1</v>
@@ -7269,11 +7270,11 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">B18+Constrained_Data!C23</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>4</v>
@@ -7287,11 +7288,11 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">B19+Constrained_Data!C24</f>
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>4</v>
@@ -7305,11 +7306,11 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">B20+Constrained_Data!C25</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>2</v>
@@ -7323,11 +7324,11 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">B21+Constrained_Data!C26</f>
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>2</v>
@@ -7341,11 +7342,11 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">B22+Constrained_Data!C27</f>
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>4</v>
@@ -7359,11 +7360,11 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">B23+Constrained_Data!C28</f>
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>1</v>
@@ -7377,11 +7378,11 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">B24+Constrained_Data!C29</f>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>1</v>
@@ -7395,11 +7396,11 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">B25+Constrained_Data!C30</f>
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>2</v>
@@ -7413,11 +7414,11 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">B26+Constrained_Data!C31</f>
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>1</v>
@@ -7449,11 +7450,11 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">B28+Constrained_Data!C33</f>
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>4</v>
@@ -7467,11 +7468,11 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">B29+Constrained_Data!C34</f>
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>2</v>
@@ -7485,11 +7486,11 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">B30+Constrained_Data!C35</f>
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>2</v>
@@ -7521,11 +7522,11 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">B32+Constrained_Data!C37</f>
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
With results for all six preliminary conditions
</commit_message>
<xml_diff>
--- a/J301_1_Manual_Calcs.xlsx
+++ b/J301_1_Manual_Calcs.xlsx
@@ -20,8 +20,12 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -410,14 +414,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.87441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.13953488372093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.24651162790698"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.38604651162791"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.06046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10697674418605"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="2.58604651162791"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5813953488372"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.58604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1337,8 +1343,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,14 +1797,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.87441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.13953488372093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.24651162790698"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.38604651162791"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="3.2"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.093023255814"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="3.2"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="3.44651162790698"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="3.44651162790698"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2786,11 +2794,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.87441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.13953488372093"/>
-    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.24651162790698"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5202,18 +5211,19 @@
   <dimension ref="A1:CU33"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="0" topLeftCell="AG1" activePane="topRight" state="frozen"/>
+      <pane xSplit="6" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B33" activeCellId="0" sqref="B33"/>
+      <selection pane="topRight" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.87441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.13953488372093"/>
-    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.24651162790698"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5531,43 +5541,43 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; I$1,$C$2:$C$33,"&gt;" &amp; I$1)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; J$1,$C$2:$C$33,"&gt;" &amp; J$1)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; K$1,$C$2:$C$33,"&gt;" &amp; K$1)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; L$1,$C$2:$C$33,"&gt;" &amp; L$1)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; M$1,$C$2:$C$33,"&gt;" &amp; M$1)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; N$1,$C$2:$C$33,"&gt;" &amp; N$1)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; O$1,$C$2:$C$33,"&gt;" &amp; O$1)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; P$1,$C$2:$C$33,"&gt;" &amp; P$1)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; Q$1,$C$2:$C$33,"&gt;" &amp; Q$1)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="R2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; R$1,$C$2:$C$33,"&gt;" &amp; R$1)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="S2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; S$1,$C$2:$C$33,"&gt;" &amp; S$1)</f>
@@ -5579,59 +5589,59 @@
       </c>
       <c r="U2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="V2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="W2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; W$1,$C$2:$C$33,"&gt;" &amp; W$1)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="X2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; X$1,$C$2:$C$33,"&gt;" &amp; X$1)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Y2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; Y$1,$C$2:$C$33,"&gt;" &amp; Y$1)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Z2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AA2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AB2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AC2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AD2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AF2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AI2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
@@ -5643,19 +5653,19 @@
       </c>
       <c r="AK2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AM2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AN2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
@@ -5671,27 +5681,27 @@
       </c>
       <c r="AR2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AR$1,$C$2:$C$33,"&gt;" &amp; AR$1)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AS2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AS$1,$C$2:$C$33,"&gt;" &amp; AS$1)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AT2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AT$1,$C$2:$C$33,"&gt;" &amp; AT$1)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AU2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AU$1,$C$2:$C$33,"&gt;" &amp; AU$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AV2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AX2" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
@@ -5899,11 +5909,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">B3+Constrained_Data!C8</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>1</v>
@@ -5932,35 +5942,35 @@
       </c>
       <c r="M3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; M$1,$C$2:$C$33,"&gt;" &amp; M$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; N$1,$C$2:$C$33,"&gt;" &amp; N$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; O$1,$C$2:$C$33,"&gt;" &amp; O$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; P$1,$C$2:$C$33,"&gt;" &amp; P$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; Q$1,$C$2:$C$33,"&gt;" &amp; Q$1)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; R$1,$C$2:$C$33,"&gt;" &amp; R$1)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; S$1,$C$2:$C$33,"&gt;" &amp; S$1)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; T$1,$C$2:$C$33,"&gt;" &amp; T$1)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
@@ -5968,11 +5978,11 @@
       </c>
       <c r="V3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="W3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; W$1,$C$2:$C$33,"&gt;" &amp; W$1)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="X3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; X$1,$C$2:$C$33,"&gt;" &amp; X$1)</f>
@@ -5980,79 +5990,79 @@
       </c>
       <c r="Y3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; Y$1,$C$2:$C$33,"&gt;" &amp; Y$1)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="Z3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="AA3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="AB3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AC3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AD3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AE3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AF3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AG3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AH3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AI3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AJ3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AL3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AM3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AN3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AO3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AP3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AQ3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AQ$1,$C$2:$C$33,"&gt;" &amp; AQ$1)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AR3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AR$1,$C$2:$C$33,"&gt;" &amp; AR$1)</f>
@@ -6068,39 +6078,39 @@
       </c>
       <c r="AU3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AU$1,$C$2:$C$33,"&gt;" &amp; AU$1)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AV3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AW3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AX3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AY3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AZ3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BA3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="BB3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="BC3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="BD3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
@@ -6112,31 +6122,31 @@
       </c>
       <c r="BF3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BG3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BG$1,$C$2:$C$33,"&gt;" &amp; BG$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BH3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BH$1,$C$2:$C$33,"&gt;" &amp; BH$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BI3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BI$1,$C$2:$C$33,"&gt;" &amp; BI$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BJ3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BJ$1,$C$2:$C$33,"&gt;" &amp; BJ$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BK3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BK$1,$C$2:$C$33,"&gt;" &amp; BK$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BL3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BL$1,$C$2:$C$33,"&gt;" &amp; BL$1)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BM3" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BM$1,$C$2:$C$33,"&gt;" &amp; BM$1)</f>
@@ -6284,11 +6294,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">B4+Constrained_Data!C9</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>1</v>
@@ -6369,19 +6379,19 @@
       </c>
       <c r="Z4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
@@ -6397,19 +6407,19 @@
       </c>
       <c r="AG4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AI4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AJ4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AK4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
@@ -6477,11 +6487,11 @@
       </c>
       <c r="BA4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BB4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
@@ -6489,11 +6499,11 @@
       </c>
       <c r="BD4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BE4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF4" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
@@ -6718,43 +6728,43 @@
       </c>
       <c r="Q5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; Q$1,$C$2:$C$33,"&gt;" &amp; Q$1)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="R5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; R$1,$C$2:$C$33,"&gt;" &amp; R$1)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="S5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; S$1,$C$2:$C$33,"&gt;" &amp; S$1)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="T5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; T$1,$C$2:$C$33,"&gt;" &amp; T$1)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="U5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="V5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="W5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; W$1,$C$2:$C$33,"&gt;" &amp; W$1)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="X5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; X$1,$C$2:$C$33,"&gt;" &amp; X$1)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="Y5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; Y$1,$C$2:$C$33,"&gt;" &amp; Y$1)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Z5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AA5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
@@ -6778,23 +6788,23 @@
       </c>
       <c r="AF5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AG5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AH5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AI5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AJ5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AK5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
@@ -6802,23 +6812,23 @@
       </c>
       <c r="AL5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AN5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AO5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AP5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AQ5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AQ$1,$C$2:$C$33,"&gt;" &amp; AQ$1)</f>
@@ -6834,43 +6844,43 @@
       </c>
       <c r="AT5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AT$1,$C$2:$C$33,"&gt;" &amp; AT$1)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AU5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AU$1,$C$2:$C$33,"&gt;" &amp; AU$1)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AV5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AW5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AX5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AY5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AZ5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BA5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BB5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BC5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BD5" s="0" t="n">
         <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
@@ -7072,11 +7082,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">B7+Constrained_Data!C12</f>
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>4</v>
@@ -7108,11 +7118,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">B9+Constrained_Data!C14</f>
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>2</v>
@@ -7126,11 +7136,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">B10+Constrained_Data!C15</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>1</v>
@@ -7162,11 +7172,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">B12+Constrained_Data!C17</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>2</v>
@@ -7180,11 +7190,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">B13+Constrained_Data!C18</f>
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>2</v>
@@ -7198,11 +7208,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">B14+Constrained_Data!C19</f>
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>1</v>
@@ -7216,11 +7226,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">B15+Constrained_Data!C20</f>
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>2</v>
@@ -7234,11 +7244,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">B16+Constrained_Data!C21</f>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>1</v>
@@ -7252,11 +7262,11 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">B17+Constrained_Data!C22</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>4</v>
@@ -7270,11 +7280,11 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">B18+Constrained_Data!C23</f>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>4</v>
@@ -7288,11 +7298,11 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">B19+Constrained_Data!C24</f>
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>4</v>
@@ -7306,11 +7316,11 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">B20+Constrained_Data!C25</f>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>2</v>
@@ -7324,11 +7334,11 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">B21+Constrained_Data!C26</f>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>2</v>
@@ -7342,11 +7352,11 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">B22+Constrained_Data!C27</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>4</v>
@@ -7360,11 +7370,11 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">B23+Constrained_Data!C28</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>1</v>
@@ -7378,11 +7388,11 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">B24+Constrained_Data!C29</f>
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>1</v>
@@ -7396,11 +7406,11 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">B25+Constrained_Data!C30</f>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>2</v>
@@ -7414,11 +7424,11 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">B26+Constrained_Data!C31</f>
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>1</v>
@@ -7432,11 +7442,11 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">B27+Constrained_Data!C32</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>3</v>
@@ -7450,11 +7460,11 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">B28+Constrained_Data!C33</f>
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>4</v>
@@ -7468,11 +7478,11 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">B29+Constrained_Data!C34</f>
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>2</v>
@@ -7486,11 +7496,11 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">B30+Constrained_Data!C35</f>
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>2</v>
@@ -7504,11 +7514,11 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">B31+Constrained_Data!C36</f>
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>2</v>
@@ -7522,11 +7532,11 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">B32+Constrained_Data!C37</f>
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>3</v>
@@ -7540,11 +7550,11 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">B33+Constrained_Data!C38</f>
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Added script to check for files with multiple resources per task
</commit_message>
<xml_diff>
--- a/J301_1_Manual_Calcs.xlsx
+++ b/J301_1_Manual_Calcs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,19 +13,23 @@
     <sheet name="Constrained_Data" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="By_Task_Num" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="By_Task_Num_Auto" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="By_Task_Num_Auto_2" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num_Auto_2!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">By_Task_Num!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">By_Task_Num_Auto!$A$1:$E$33</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="49">
   <si>
     <t>Resources</t>
   </si>
@@ -401,6 +405,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -414,16 +422,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.24651162790698"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.50697674418605"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.35348837209302"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="2.58604651162791"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8279069767442"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.58604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,8 +1351,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,16 +1805,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.24651162790698"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.50697674418605"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="3.44651162790698"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="3.44651162790698"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="3.56744186046512"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="3.56744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,12 +2802,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.24651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.38604651162791"/>
-    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.50697674418605"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5210,7 +5218,7 @@
   </sheetPr>
   <dimension ref="A1:CU33"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B22" activeCellId="0" sqref="B22"/>
@@ -5218,12 +5226,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.24651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.38604651162791"/>
-    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.50697674418605"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7594,4 +7602,2365 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:CU33"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="L6" activeCellId="0" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.50697674418605"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.093023255814"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="S1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="T1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="U1" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="V1" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="W1" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="X1" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y1" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z1" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA1" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AB1" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC1" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD1" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE1" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="AG1" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AH1" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AI1" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="AJ1" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AK1" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AL1" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AM1" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AN1" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AO1" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AP1" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ1" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="AR1" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AS1" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="AT1" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="AU1" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="AV1" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="AW1" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AX1" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="AY1" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AZ1" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="BA1" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="BB1" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="BC1" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="BD1" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="BE1" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="BF1" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="BG1" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="BH1" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="BI1" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="BJ1" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="BK1" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="BL1" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="BM1" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="BN1" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="BO1" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="BP1" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="BQ1" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="BR1" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="BS1" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="BT1" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="BU1" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="BV1" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="BW1" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="BX1" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="BY1" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="BZ1" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="CA1" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="CB1" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="CC1" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="CD1" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="CE1" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="CF1" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="CG1" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="CH1" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="CI1" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="CJ1" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="CK1" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="CL1" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="CM1" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="CN1" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="CO1" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="CP1" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="CQ1" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="CR1" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="CS1" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="CT1" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="CU1" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; I$1,$C$2:$C$33,"&gt;" &amp; I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; J$1,$C$2:$C$33,"&gt;" &amp; J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; K$1,$C$2:$C$33,"&gt;" &amp; K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; L$1,$C$2:$C$33,"&gt;" &amp; L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; M$1,$C$2:$C$33,"&gt;" &amp; M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; N$1,$C$2:$C$33,"&gt;" &amp; N$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; O$1,$C$2:$C$33,"&gt;" &amp; O$1)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; P$1,$C$2:$C$33,"&gt;" &amp; P$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; Q$1,$C$2:$C$33,"&gt;" &amp; Q$1)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; R$1,$C$2:$C$33,"&gt;" &amp; R$1)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; S$1,$C$2:$C$33,"&gt;" &amp; S$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; T$1,$C$2:$C$33,"&gt;" &amp; T$1)</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
+        <v>0</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; W$1,$C$2:$C$33,"&gt;" &amp; W$1)</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; X$1,$C$2:$C$33,"&gt;" &amp; X$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; Y$1,$C$2:$C$33,"&gt;" &amp; Y$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
+        <v>4</v>
+      </c>
+      <c r="AC2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
+        <v>4</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
+        <v>4</v>
+      </c>
+      <c r="AE2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
+        <v>4</v>
+      </c>
+      <c r="AF2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
+        <v>4</v>
+      </c>
+      <c r="AG2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
+        <v>4</v>
+      </c>
+      <c r="AH2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
+        <v>4</v>
+      </c>
+      <c r="AI2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
+        <v>4</v>
+      </c>
+      <c r="AK2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
+        <v>9</v>
+      </c>
+      <c r="AL2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
+        <v>9</v>
+      </c>
+      <c r="AM2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
+        <v>9</v>
+      </c>
+      <c r="AN2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
+        <v>9</v>
+      </c>
+      <c r="AO2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AP2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AQ$1,$C$2:$C$33,"&gt;" &amp; AQ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AR2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AR$1,$C$2:$C$33,"&gt;" &amp; AR$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AS2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AS$1,$C$2:$C$33,"&gt;" &amp; AS$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AT2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AT$1,$C$2:$C$33,"&gt;" &amp; AT$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AU2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AU$1,$C$2:$C$33,"&gt;" &amp; AU$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AV2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AW2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AX2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AY2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BA2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BB2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BC2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BD2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BE2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BF2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BG2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BG$1,$C$2:$C$33,"&gt;" &amp; BG$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BH2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BH$1,$C$2:$C$33,"&gt;" &amp; BH$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BI2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BI$1,$C$2:$C$33,"&gt;" &amp; BI$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BJ2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BJ$1,$C$2:$C$33,"&gt;" &amp; BJ$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BK2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BK$1,$C$2:$C$33,"&gt;" &amp; BK$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BL2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BL$1,$C$2:$C$33,"&gt;" &amp; BL$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BM2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BM$1,$C$2:$C$33,"&gt;" &amp; BM$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BN2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BN$1,$C$2:$C$33,"&gt;" &amp; BN$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BO2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BO$1,$C$2:$C$33,"&gt;" &amp; BO$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BP2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BP$1,$C$2:$C$33,"&gt;" &amp; BP$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BQ$1,$C$2:$C$33,"&gt;" &amp; BQ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BR2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BR$1,$C$2:$C$33,"&gt;" &amp; BR$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BS2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BS$1,$C$2:$C$33,"&gt;" &amp; BS$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BT2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BT$1,$C$2:$C$33,"&gt;" &amp; BT$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BU2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BU$1,$C$2:$C$33,"&gt;" &amp; BU$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BV2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BV$1,$C$2:$C$33,"&gt;" &amp; BV$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BW2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BW$1,$C$2:$C$33,"&gt;" &amp; BW$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BX2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BX$1,$C$2:$C$33,"&gt;" &amp; BX$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BY2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BY$1,$C$2:$C$33,"&gt;" &amp; BY$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BZ2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; BZ$1,$C$2:$C$33,"&gt;" &amp; BZ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CA2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CA$1,$C$2:$C$33,"&gt;" &amp; CA$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CB2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CB$1,$C$2:$C$33,"&gt;" &amp; CB$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CC2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CC$1,$C$2:$C$33,"&gt;" &amp; CC$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CD2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CD$1,$C$2:$C$33,"&gt;" &amp; CD$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CE2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CE$1,$C$2:$C$33,"&gt;" &amp; CE$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CF2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CF$1,$C$2:$C$33,"&gt;" &amp; CF$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CG2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CG$1,$C$2:$C$33,"&gt;" &amp; CG$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CH2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CH$1,$C$2:$C$33,"&gt;" &amp; CH$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CI2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CI$1,$C$2:$C$33,"&gt;" &amp; CI$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CJ2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CJ$1,$C$2:$C$33,"&gt;" &amp; CJ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CK2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CK$1,$C$2:$C$33,"&gt;" &amp; CK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CL2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CL$1,$C$2:$C$33,"&gt;" &amp; CL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CM2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CM$1,$C$2:$C$33,"&gt;" &amp; CM$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CN2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CN$1,$C$2:$C$33,"&gt;" &amp; CN$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CO2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CO$1,$C$2:$C$33,"&gt;" &amp; CO$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CP2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CP$1,$C$2:$C$33,"&gt;" &amp; CP$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CQ2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CQ$1,$C$2:$C$33,"&gt;" &amp; CQ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CR2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CR$1,$C$2:$C$33,"&gt;" &amp; CR$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CS2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CS$1,$C$2:$C$33,"&gt;" &amp; CS$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CT2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CT$1,$C$2:$C$33,"&gt;" &amp; CT$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CU2" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H2,$B$2:$B$33,"&lt;=" &amp; CU$1,$C$2:$C$33,"&gt;" &amp; CU$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; I$1,$C$2:$C$33,"&gt;" &amp; I$1)</f>
+        <v>10</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; J$1,$C$2:$C$33,"&gt;" &amp; J$1)</f>
+        <v>10</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; K$1,$C$2:$C$33,"&gt;" &amp; K$1)</f>
+        <v>10</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; L$1,$C$2:$C$33,"&gt;" &amp; L$1)</f>
+        <v>10</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; M$1,$C$2:$C$33,"&gt;" &amp; M$1)</f>
+        <v>10</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; N$1,$C$2:$C$33,"&gt;" &amp; N$1)</f>
+        <v>10</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; O$1,$C$2:$C$33,"&gt;" &amp; O$1)</f>
+        <v>10</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; P$1,$C$2:$C$33,"&gt;" &amp; P$1)</f>
+        <v>10</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; Q$1,$C$2:$C$33,"&gt;" &amp; Q$1)</f>
+        <v>10</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; R$1,$C$2:$C$33,"&gt;" &amp; R$1)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; S$1,$C$2:$C$33,"&gt;" &amp; S$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; T$1,$C$2:$C$33,"&gt;" &amp; T$1)</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
+        <v>0</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; W$1,$C$2:$C$33,"&gt;" &amp; W$1)</f>
+        <v>0</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; X$1,$C$2:$C$33,"&gt;" &amp; X$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; Y$1,$C$2:$C$33,"&gt;" &amp; Y$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AD3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AE3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AF3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AG3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AH3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AI3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AK3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AL3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AN3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AP3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AQ$1,$C$2:$C$33,"&gt;" &amp; AQ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AR3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AR$1,$C$2:$C$33,"&gt;" &amp; AR$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AS3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AS$1,$C$2:$C$33,"&gt;" &amp; AS$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AT3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AT$1,$C$2:$C$33,"&gt;" &amp; AT$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AU3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AU$1,$C$2:$C$33,"&gt;" &amp; AU$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AV3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AW3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AX3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AY3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
+        <v>5</v>
+      </c>
+      <c r="AZ3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BA3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BB3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BC3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BD3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BE3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BF3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BG3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BG$1,$C$2:$C$33,"&gt;" &amp; BG$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BH3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BH$1,$C$2:$C$33,"&gt;" &amp; BH$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BI3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BI$1,$C$2:$C$33,"&gt;" &amp; BI$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BJ$1,$C$2:$C$33,"&gt;" &amp; BJ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BK3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BK$1,$C$2:$C$33,"&gt;" &amp; BK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BL3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BL$1,$C$2:$C$33,"&gt;" &amp; BL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BM3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BM$1,$C$2:$C$33,"&gt;" &amp; BM$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BN3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BN$1,$C$2:$C$33,"&gt;" &amp; BN$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BO3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BO$1,$C$2:$C$33,"&gt;" &amp; BO$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BP3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BP$1,$C$2:$C$33,"&gt;" &amp; BP$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BQ$1,$C$2:$C$33,"&gt;" &amp; BQ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BR3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BR$1,$C$2:$C$33,"&gt;" &amp; BR$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BS3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BS$1,$C$2:$C$33,"&gt;" &amp; BS$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BT3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BT$1,$C$2:$C$33,"&gt;" &amp; BT$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BU3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BU$1,$C$2:$C$33,"&gt;" &amp; BU$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BV3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BV$1,$C$2:$C$33,"&gt;" &amp; BV$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BW3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BW$1,$C$2:$C$33,"&gt;" &amp; BW$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BX3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BX$1,$C$2:$C$33,"&gt;" &amp; BX$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BY3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BY$1,$C$2:$C$33,"&gt;" &amp; BY$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BZ3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; BZ$1,$C$2:$C$33,"&gt;" &amp; BZ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CA3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CA$1,$C$2:$C$33,"&gt;" &amp; CA$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CB3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CB$1,$C$2:$C$33,"&gt;" &amp; CB$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CC3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CC$1,$C$2:$C$33,"&gt;" &amp; CC$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CD3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CD$1,$C$2:$C$33,"&gt;" &amp; CD$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CE3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CE$1,$C$2:$C$33,"&gt;" &amp; CE$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CF3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CF$1,$C$2:$C$33,"&gt;" &amp; CF$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CG3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CG$1,$C$2:$C$33,"&gt;" &amp; CG$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CH3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CH$1,$C$2:$C$33,"&gt;" &amp; CH$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CI3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CI$1,$C$2:$C$33,"&gt;" &amp; CI$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CJ3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CJ$1,$C$2:$C$33,"&gt;" &amp; CJ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CK3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CK$1,$C$2:$C$33,"&gt;" &amp; CK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CL3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CL$1,$C$2:$C$33,"&gt;" &amp; CL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CM3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CM$1,$C$2:$C$33,"&gt;" &amp; CM$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CN3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CN$1,$C$2:$C$33,"&gt;" &amp; CN$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CO3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CO$1,$C$2:$C$33,"&gt;" &amp; CO$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CP3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CP$1,$C$2:$C$33,"&gt;" &amp; CP$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CQ3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CQ$1,$C$2:$C$33,"&gt;" &amp; CQ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CR3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CR$1,$C$2:$C$33,"&gt;" &amp; CR$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CS3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CS$1,$C$2:$C$33,"&gt;" &amp; CS$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CT3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CT$1,$C$2:$C$33,"&gt;" &amp; CT$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CU3" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H3,$B$2:$B$33,"&lt;=" &amp; CU$1,$C$2:$C$33,"&gt;" &amp; CU$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; I$1,$C$2:$C$33,"&gt;" &amp; I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; J$1,$C$2:$C$33,"&gt;" &amp; J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; K$1,$C$2:$C$33,"&gt;" &amp; K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; L$1,$C$2:$C$33,"&gt;" &amp; L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; M$1,$C$2:$C$33,"&gt;" &amp; M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; N$1,$C$2:$C$33,"&gt;" &amp; N$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; O$1,$C$2:$C$33,"&gt;" &amp; O$1)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; P$1,$C$2:$C$33,"&gt;" &amp; P$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; Q$1,$C$2:$C$33,"&gt;" &amp; Q$1)</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; R$1,$C$2:$C$33,"&gt;" &amp; R$1)</f>
+        <v>13</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; S$1,$C$2:$C$33,"&gt;" &amp; S$1)</f>
+        <v>13</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; T$1,$C$2:$C$33,"&gt;" &amp; T$1)</f>
+        <v>13</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
+        <v>11</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
+        <v>11</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; W$1,$C$2:$C$33,"&gt;" &amp; W$1)</f>
+        <v>11</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; X$1,$C$2:$C$33,"&gt;" &amp; X$1)</f>
+        <v>11</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; Y$1,$C$2:$C$33,"&gt;" &amp; Y$1)</f>
+        <v>11</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
+        <v>2</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
+        <v>2</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
+        <v>1</v>
+      </c>
+      <c r="AF4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AG4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AI4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AK4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AL4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AM4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AN4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AO4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AP4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AQ4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AQ$1,$C$2:$C$33,"&gt;" &amp; AQ$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AR4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AR$1,$C$2:$C$33,"&gt;" &amp; AR$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AS4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AS$1,$C$2:$C$33,"&gt;" &amp; AS$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AT4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AT$1,$C$2:$C$33,"&gt;" &amp; AT$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AU4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AU$1,$C$2:$C$33,"&gt;" &amp; AU$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AV4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AW4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AX4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
+        <v>9</v>
+      </c>
+      <c r="AY4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
+        <v>9</v>
+      </c>
+      <c r="AZ4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
+        <v>9</v>
+      </c>
+      <c r="BA4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
+        <v>9</v>
+      </c>
+      <c r="BB4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
+        <v>9</v>
+      </c>
+      <c r="BC4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
+        <v>9</v>
+      </c>
+      <c r="BD4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
+        <v>9</v>
+      </c>
+      <c r="BE4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
+        <v>9</v>
+      </c>
+      <c r="BF4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
+        <v>15</v>
+      </c>
+      <c r="BG4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BG$1,$C$2:$C$33,"&gt;" &amp; BG$1)</f>
+        <v>15</v>
+      </c>
+      <c r="BH4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BH$1,$C$2:$C$33,"&gt;" &amp; BH$1)</f>
+        <v>8</v>
+      </c>
+      <c r="BI4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BI$1,$C$2:$C$33,"&gt;" &amp; BI$1)</f>
+        <v>8</v>
+      </c>
+      <c r="BJ4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BJ$1,$C$2:$C$33,"&gt;" &amp; BJ$1)</f>
+        <v>8</v>
+      </c>
+      <c r="BK4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BK$1,$C$2:$C$33,"&gt;" &amp; BK$1)</f>
+        <v>8</v>
+      </c>
+      <c r="BL4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BL$1,$C$2:$C$33,"&gt;" &amp; BL$1)</f>
+        <v>8</v>
+      </c>
+      <c r="BM4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BM$1,$C$2:$C$33,"&gt;" &amp; BM$1)</f>
+        <v>14</v>
+      </c>
+      <c r="BN4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BN$1,$C$2:$C$33,"&gt;" &amp; BN$1)</f>
+        <v>14</v>
+      </c>
+      <c r="BO4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BO$1,$C$2:$C$33,"&gt;" &amp; BO$1)</f>
+        <v>14</v>
+      </c>
+      <c r="BP4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BP$1,$C$2:$C$33,"&gt;" &amp; BP$1)</f>
+        <v>14</v>
+      </c>
+      <c r="BQ4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BQ$1,$C$2:$C$33,"&gt;" &amp; BQ$1)</f>
+        <v>14</v>
+      </c>
+      <c r="BR4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BR$1,$C$2:$C$33,"&gt;" &amp; BR$1)</f>
+        <v>14</v>
+      </c>
+      <c r="BS4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BS$1,$C$2:$C$33,"&gt;" &amp; BS$1)</f>
+        <v>15</v>
+      </c>
+      <c r="BT4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BT$1,$C$2:$C$33,"&gt;" &amp; BT$1)</f>
+        <v>6</v>
+      </c>
+      <c r="BU4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BU$1,$C$2:$C$33,"&gt;" &amp; BU$1)</f>
+        <v>6</v>
+      </c>
+      <c r="BV4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BV$1,$C$2:$C$33,"&gt;" &amp; BV$1)</f>
+        <v>4</v>
+      </c>
+      <c r="BW4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BW$1,$C$2:$C$33,"&gt;" &amp; BW$1)</f>
+        <v>4</v>
+      </c>
+      <c r="BX4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BX$1,$C$2:$C$33,"&gt;" &amp; BX$1)</f>
+        <v>4</v>
+      </c>
+      <c r="BY4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BY$1,$C$2:$C$33,"&gt;" &amp; BY$1)</f>
+        <v>4</v>
+      </c>
+      <c r="BZ4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; BZ$1,$C$2:$C$33,"&gt;" &amp; BZ$1)</f>
+        <v>4</v>
+      </c>
+      <c r="CA4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CA$1,$C$2:$C$33,"&gt;" &amp; CA$1)</f>
+        <v>4</v>
+      </c>
+      <c r="CB4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CB$1,$C$2:$C$33,"&gt;" &amp; CB$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CC4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CC$1,$C$2:$C$33,"&gt;" &amp; CC$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CD4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CD$1,$C$2:$C$33,"&gt;" &amp; CD$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CE4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CE$1,$C$2:$C$33,"&gt;" &amp; CE$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CF4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CF$1,$C$2:$C$33,"&gt;" &amp; CF$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CG4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CG$1,$C$2:$C$33,"&gt;" &amp; CG$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CH4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CH$1,$C$2:$C$33,"&gt;" &amp; CH$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CI4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CI$1,$C$2:$C$33,"&gt;" &amp; CI$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CJ4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CJ$1,$C$2:$C$33,"&gt;" &amp; CJ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CK4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CK$1,$C$2:$C$33,"&gt;" &amp; CK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CL4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CL$1,$C$2:$C$33,"&gt;" &amp; CL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CM4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CM$1,$C$2:$C$33,"&gt;" &amp; CM$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CN4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CN$1,$C$2:$C$33,"&gt;" &amp; CN$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CO4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CO$1,$C$2:$C$33,"&gt;" &amp; CO$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CP4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CP$1,$C$2:$C$33,"&gt;" &amp; CP$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CQ4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CQ$1,$C$2:$C$33,"&gt;" &amp; CQ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CR4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CR$1,$C$2:$C$33,"&gt;" &amp; CR$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CS4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CS$1,$C$2:$C$33,"&gt;" &amp; CS$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CT4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CT$1,$C$2:$C$33,"&gt;" &amp; CT$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CU4" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H4,$B$2:$B$33,"&lt;=" &amp; CU$1,$C$2:$C$33,"&gt;" &amp; CU$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; I$1,$C$2:$C$33,"&gt;" &amp; I$1)</f>
+        <v>10</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; J$1,$C$2:$C$33,"&gt;" &amp; J$1)</f>
+        <v>10</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; K$1,$C$2:$C$33,"&gt;" &amp; K$1)</f>
+        <v>10</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; L$1,$C$2:$C$33,"&gt;" &amp; L$1)</f>
+        <v>10</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; M$1,$C$2:$C$33,"&gt;" &amp; M$1)</f>
+        <v>10</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; N$1,$C$2:$C$33,"&gt;" &amp; N$1)</f>
+        <v>10</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; O$1,$C$2:$C$33,"&gt;" &amp; O$1)</f>
+        <v>10</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; P$1,$C$2:$C$33,"&gt;" &amp; P$1)</f>
+        <v>10</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; Q$1,$C$2:$C$33,"&gt;" &amp; Q$1)</f>
+        <v>10</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; R$1,$C$2:$C$33,"&gt;" &amp; R$1)</f>
+        <v>9</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; S$1,$C$2:$C$33,"&gt;" &amp; S$1)</f>
+        <v>9</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; T$1,$C$2:$C$33,"&gt;" &amp; T$1)</f>
+        <v>9</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; U$1,$C$2:$C$33,"&gt;" &amp; U$1)</f>
+        <v>9</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; V$1,$C$2:$C$33,"&gt;" &amp; V$1)</f>
+        <v>9</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; W$1,$C$2:$C$33,"&gt;" &amp; W$1)</f>
+        <v>7</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; X$1,$C$2:$C$33,"&gt;" &amp; X$1)</f>
+        <v>7</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; Y$1,$C$2:$C$33,"&gt;" &amp; Y$1)</f>
+        <v>7</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; Z$1,$C$2:$C$33,"&gt;" &amp; Z$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AA$1,$C$2:$C$33,"&gt;" &amp; AA$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AB$1,$C$2:$C$33,"&gt;" &amp; AB$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AC$1,$C$2:$C$33,"&gt;" &amp; AC$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AD$1,$C$2:$C$33,"&gt;" &amp; AD$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AE$1,$C$2:$C$33,"&gt;" &amp; AE$1)</f>
+        <v>5</v>
+      </c>
+      <c r="AF5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AF$1,$C$2:$C$33,"&gt;" &amp; AF$1)</f>
+        <v>5</v>
+      </c>
+      <c r="AG5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AG$1,$C$2:$C$33,"&gt;" &amp; AG$1)</f>
+        <v>5</v>
+      </c>
+      <c r="AH5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AH$1,$C$2:$C$33,"&gt;" &amp; AH$1)</f>
+        <v>5</v>
+      </c>
+      <c r="AI5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AI$1,$C$2:$C$33,"&gt;" &amp; AI$1)</f>
+        <v>5</v>
+      </c>
+      <c r="AJ5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AJ$1,$C$2:$C$33,"&gt;" &amp; AJ$1)</f>
+        <v>5</v>
+      </c>
+      <c r="AK5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AK$1,$C$2:$C$33,"&gt;" &amp; AK$1)</f>
+        <v>10</v>
+      </c>
+      <c r="AL5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AL$1,$C$2:$C$33,"&gt;" &amp; AL$1)</f>
+        <v>10</v>
+      </c>
+      <c r="AM5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AM$1,$C$2:$C$33,"&gt;" &amp; AM$1)</f>
+        <v>10</v>
+      </c>
+      <c r="AN5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AN$1,$C$2:$C$33,"&gt;" &amp; AN$1)</f>
+        <v>7</v>
+      </c>
+      <c r="AO5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AO$1,$C$2:$C$33,"&gt;" &amp; AO$1)</f>
+        <v>3</v>
+      </c>
+      <c r="AP5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AP$1,$C$2:$C$33,"&gt;" &amp; AP$1)</f>
+        <v>3</v>
+      </c>
+      <c r="AQ5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AQ$1,$C$2:$C$33,"&gt;" &amp; AQ$1)</f>
+        <v>3</v>
+      </c>
+      <c r="AR5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AR$1,$C$2:$C$33,"&gt;" &amp; AR$1)</f>
+        <v>3</v>
+      </c>
+      <c r="AS5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AS$1,$C$2:$C$33,"&gt;" &amp; AS$1)</f>
+        <v>3</v>
+      </c>
+      <c r="AT5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AT$1,$C$2:$C$33,"&gt;" &amp; AT$1)</f>
+        <v>3</v>
+      </c>
+      <c r="AU5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AU$1,$C$2:$C$33,"&gt;" &amp; AU$1)</f>
+        <v>3</v>
+      </c>
+      <c r="AV5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AV$1,$C$2:$C$33,"&gt;" &amp; AV$1)</f>
+        <v>3</v>
+      </c>
+      <c r="AW5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AW$1,$C$2:$C$33,"&gt;" &amp; AW$1)</f>
+        <v>3</v>
+      </c>
+      <c r="AX5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AX$1,$C$2:$C$33,"&gt;" &amp; AX$1)</f>
+        <v>9</v>
+      </c>
+      <c r="AY5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AY$1,$C$2:$C$33,"&gt;" &amp; AY$1)</f>
+        <v>8</v>
+      </c>
+      <c r="AZ5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; AZ$1,$C$2:$C$33,"&gt;" &amp; AZ$1)</f>
+        <v>8</v>
+      </c>
+      <c r="BA5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BA$1,$C$2:$C$33,"&gt;" &amp; BA$1)</f>
+        <v>8</v>
+      </c>
+      <c r="BB5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BB$1,$C$2:$C$33,"&gt;" &amp; BB$1)</f>
+        <v>8</v>
+      </c>
+      <c r="BC5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BC$1,$C$2:$C$33,"&gt;" &amp; BC$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BD5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BD$1,$C$2:$C$33,"&gt;" &amp; BD$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BE5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BE$1,$C$2:$C$33,"&gt;" &amp; BE$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BF5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BF$1,$C$2:$C$33,"&gt;" &amp; BF$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BG5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BG$1,$C$2:$C$33,"&gt;" &amp; BG$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BH5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BH$1,$C$2:$C$33,"&gt;" &amp; BH$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BI5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BI$1,$C$2:$C$33,"&gt;" &amp; BI$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BJ5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BJ$1,$C$2:$C$33,"&gt;" &amp; BJ$1)</f>
+        <v>7</v>
+      </c>
+      <c r="BK5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BK$1,$C$2:$C$33,"&gt;" &amp; BK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BL5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BL$1,$C$2:$C$33,"&gt;" &amp; BL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BM5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BM$1,$C$2:$C$33,"&gt;" &amp; BM$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BN5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BN$1,$C$2:$C$33,"&gt;" &amp; BN$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BO5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BO$1,$C$2:$C$33,"&gt;" &amp; BO$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BP5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BP$1,$C$2:$C$33,"&gt;" &amp; BP$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BQ$1,$C$2:$C$33,"&gt;" &amp; BQ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BR5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BR$1,$C$2:$C$33,"&gt;" &amp; BR$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BS5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BS$1,$C$2:$C$33,"&gt;" &amp; BS$1)</f>
+        <v>0</v>
+      </c>
+      <c r="BT5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BT$1,$C$2:$C$33,"&gt;" &amp; BT$1)</f>
+        <v>6</v>
+      </c>
+      <c r="BU5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BU$1,$C$2:$C$33,"&gt;" &amp; BU$1)</f>
+        <v>6</v>
+      </c>
+      <c r="BV5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BV$1,$C$2:$C$33,"&gt;" &amp; BV$1)</f>
+        <v>6</v>
+      </c>
+      <c r="BW5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BW$1,$C$2:$C$33,"&gt;" &amp; BW$1)</f>
+        <v>6</v>
+      </c>
+      <c r="BX5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BX$1,$C$2:$C$33,"&gt;" &amp; BX$1)</f>
+        <v>6</v>
+      </c>
+      <c r="BY5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BY$1,$C$2:$C$33,"&gt;" &amp; BY$1)</f>
+        <v>6</v>
+      </c>
+      <c r="BZ5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; BZ$1,$C$2:$C$33,"&gt;" &amp; BZ$1)</f>
+        <v>6</v>
+      </c>
+      <c r="CA5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CA$1,$C$2:$C$33,"&gt;" &amp; CA$1)</f>
+        <v>6</v>
+      </c>
+      <c r="CB5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CB$1,$C$2:$C$33,"&gt;" &amp; CB$1)</f>
+        <v>6</v>
+      </c>
+      <c r="CC5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CC$1,$C$2:$C$33,"&gt;" &amp; CC$1)</f>
+        <v>6</v>
+      </c>
+      <c r="CD5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CD$1,$C$2:$C$33,"&gt;" &amp; CD$1)</f>
+        <v>11</v>
+      </c>
+      <c r="CE5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CE$1,$C$2:$C$33,"&gt;" &amp; CE$1)</f>
+        <v>11</v>
+      </c>
+      <c r="CF5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CF$1,$C$2:$C$33,"&gt;" &amp; CF$1)</f>
+        <v>11</v>
+      </c>
+      <c r="CG5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CG$1,$C$2:$C$33,"&gt;" &amp; CG$1)</f>
+        <v>11</v>
+      </c>
+      <c r="CH5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CH$1,$C$2:$C$33,"&gt;" &amp; CH$1)</f>
+        <v>6</v>
+      </c>
+      <c r="CI5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CI$1,$C$2:$C$33,"&gt;" &amp; CI$1)</f>
+        <v>6</v>
+      </c>
+      <c r="CJ5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CJ$1,$C$2:$C$33,"&gt;" &amp; CJ$1)</f>
+        <v>6</v>
+      </c>
+      <c r="CK5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CK$1,$C$2:$C$33,"&gt;" &amp; CK$1)</f>
+        <v>6</v>
+      </c>
+      <c r="CL5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CL$1,$C$2:$C$33,"&gt;" &amp; CL$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CM5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CM$1,$C$2:$C$33,"&gt;" &amp; CM$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CN5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CN$1,$C$2:$C$33,"&gt;" &amp; CN$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CO5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CO$1,$C$2:$C$33,"&gt;" &amp; CO$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CP5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CP$1,$C$2:$C$33,"&gt;" &amp; CP$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CQ5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CQ$1,$C$2:$C$33,"&gt;" &amp; CQ$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CR5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CR$1,$C$2:$C$33,"&gt;" &amp; CR$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CS5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CS$1,$C$2:$C$33,"&gt;" &amp; CS$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CT5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CT$1,$C$2:$C$33,"&gt;" &amp; CT$1)</f>
+        <v>0</v>
+      </c>
+      <c r="CU5" s="0" t="n">
+        <f aca="false">SUMIFS($E$2:$E$33, $D$2:$D$33,$H5,$B$2:$B$33,"&lt;=" &amp; CU$1,$C$2:$C$33,"&gt;" &amp; CU$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E33"/>
+  <conditionalFormatting sqref="I5:CU5">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:CT2">
+    <cfRule type="cellIs" priority="3" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:CU3">
+    <cfRule type="cellIs" priority="4" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:CU4">
+    <cfRule type="cellIs" priority="5" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>